<commit_message>
543. Diameter of Binary Tree
543. Diameter of Binary Tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3011EC-7E21-4ABF-992B-0CC53C3F7808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6A863E-C646-4F7C-8807-06437AFE02D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Question No</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Optimal Approach</t>
+  </si>
+  <si>
+    <t>Diameter of Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -434,7 +437,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,9 +556,18 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="1">
+        <v>543</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
124. Binary Tree Maximum Path Sum
124. Binary Tree Maximum Path Sum
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6A863E-C646-4F7C-8807-06437AFE02D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B2470F-65F4-4714-961E-DE06C522121C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Question No</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Diameter of Binary Tree</t>
+  </si>
+  <si>
+    <t>Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t>Hard</t>
   </si>
 </sst>
 </file>
@@ -105,12 +111,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,7 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -153,6 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -437,7 +450,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,8 +583,21 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1">
+        <v>124</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>

<commit_message>
103. Binary Tree Zigzag Level Order Traversal
103. Binary Tree Zigzag Level Order Traversal
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B2470F-65F4-4714-961E-DE06C522121C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1026AAA6-F57C-4AD0-9E7C-1B93A7297599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2595" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>Question No</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Hard</t>
+  </si>
+  <si>
+    <t>Binary Tree Zigzag Level Order Traversal</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -111,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +127,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -138,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -166,6 +178,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -449,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,9 +613,21 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="1">
+        <v>103</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>

</xml_diff>

<commit_message>
GFG. Top View of Binary Tree
GFG. Top View of Binary Tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1026AAA6-F57C-4AD0-9E7C-1B93A7297599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D4622C-9F84-476B-9A50-CE24CFB5356E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2595" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Question No</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>GFG</t>
+  </si>
+  <si>
+    <t>Top View of Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,6 +635,20 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
     </row>

</xml_diff>

<commit_message>
GFG. Bottom view of a Binary Tree
GFG. Bottom view of a Binary Tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D4622C-9F84-476B-9A50-CE24CFB5356E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E9EA61-BE26-459F-A12A-237106E73B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2595" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Question No</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Top View of Binary Tree</t>
+  </si>
+  <si>
+    <t>Bottom View of Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,6 +654,18 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>

</xml_diff>

<commit_message>
Left and Right view of a Binary tree
Left and Right view of a Binary tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E9EA61-BE26-459F-A12A-237106E73B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0DEB2F-059B-4AAA-8300-3D3A044306C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>Question No</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>Bottom View of Binary Tree</t>
+  </si>
+  <si>
+    <t>Left View of Binary Tree</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Right View of Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -126,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +154,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -159,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -188,6 +203,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,7 +488,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,10 +683,34 @@
         <v>19</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1">
+        <v>199</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>

</xml_diff>

<commit_message>
101. Symmetric Tree or not
101. Symmetric Tree or not
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0DEB2F-059B-4AAA-8300-3D3A044306C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D6B1F-7F7A-4810-8926-04A19B27E259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>Question No</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Right View of Binary Tree</t>
+  </si>
+  <si>
+    <t>Symmetric Tree</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,6 +717,18 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
+      <c r="B15" s="1">
+        <v>101</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>

</xml_diff>

<commit_message>
4 Problem added to the list
4 Problem added to the list
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D6B1F-7F7A-4810-8926-04A19B27E259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C65A68-5254-4F0D-8F0C-0F6EE37626A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>Question No</t>
   </si>
@@ -107,6 +107,24 @@
   </si>
   <si>
     <t>Symmetric Tree</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor of a Binary Tree</t>
+  </si>
+  <si>
+    <t>Print Root to Node Path in a Binary Tree</t>
+  </si>
+  <si>
+    <t>InterviewBit</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Sum of the Longest Bloodline of a Tree</t>
+  </si>
+  <si>
+    <t>Root to Leaf Paths</t>
   </si>
 </sst>
 </file>
@@ -138,7 +156,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +181,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -177,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -207,6 +231,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -491,7 +522,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,72 +763,115 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>236</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="5"/>
     </row>

</xml_diff>

<commit_message>
Maximum width of Binary tree with 2 variations
Maximum width of Binary tree with 2 variations
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C65A68-5254-4F0D-8F0C-0F6EE37626A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F119C01-98AC-4D2E-8993-B0770B093836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Question No</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>Root to Leaf Paths</t>
+  </si>
+  <si>
+    <t>Maximum Width of Binary Tree</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>Maximum Width of Binary Tree at any level.</t>
   </si>
 </sst>
 </file>
@@ -201,7 +210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -236,6 +245,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -522,7 +534,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,13 +834,33 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="B20" s="1">
+        <v>662</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>

</xml_diff>

<commit_message>
GFG and Coding Ninja Children Sum Property
GFG and Coding Ninja Children Sum Property
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F119C01-98AC-4D2E-8993-B0770B093836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4409077F-70B0-4AFD-86DF-4D0454DE5D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
   <si>
     <t>Question No</t>
   </si>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t>Maximum Width of Binary Tree at any level.</t>
+  </si>
+  <si>
+    <t>Children Sum Property</t>
+  </si>
+  <si>
+    <t>Coding Ninja</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/childrensumproperty_790723?leftPanelTab=0</t>
+  </si>
+  <si>
+    <t>Children Sum Parent</t>
   </si>
 </sst>
 </file>
@@ -165,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +208,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -210,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -250,6 +268,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,18 +559,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="70.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="6" max="6" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -788,7 +818,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="13" t="s">
         <v>29</v>
@@ -803,7 +833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>20</v>
       </c>
@@ -817,7 +847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="13" t="s">
         <v>20</v>
@@ -832,7 +862,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>662</v>
@@ -847,7 +877,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>20</v>
@@ -862,48 +892,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="5"/>
     </row>

</xml_diff>

<commit_message>
Same Type of problem where we visit the parent node
Same Type of problem where we visit the parent node
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4409077F-70B0-4AFD-86DF-4D0454DE5D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A857C913-0414-4DF9-B5E5-5A5183815809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>Question No</t>
   </si>
@@ -146,13 +146,22 @@
   </si>
   <si>
     <t>Children Sum Parent</t>
+  </si>
+  <si>
+    <t>Time To Burn Tree</t>
+  </si>
+  <si>
+    <t>Burning Tree</t>
+  </si>
+  <si>
+    <t>All Nodes Distance K in Binary Tree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,16 +177,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +215,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -224,11 +231,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -245,7 +251,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -278,9 +283,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -562,7 +573,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,20 +659,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="7" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>104</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -675,7 +686,7 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
@@ -692,7 +703,7 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -706,10 +717,10 @@
       <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -723,10 +734,10 @@
       <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -737,10 +748,10 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -752,10 +763,10 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="11" t="s">
+      <c r="D12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -766,10 +777,10 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="12" t="s">
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -781,10 +792,10 @@
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="12" t="s">
+      <c r="D14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -796,10 +807,10 @@
       <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="12" t="s">
+      <c r="D15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -811,54 +822,54 @@
       <c r="C16" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="11" t="s">
+      <c r="D16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -873,7 +884,7 @@
       <c r="D20" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -885,57 +896,86 @@
       <c r="C21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="6"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="B25" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="B26" s="1">
+        <v>863</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>

</xml_diff>

<commit_message>
Morris Traversal- Inorder,Preorder and Flattening of Linked List
Morris Traversal- Inorder, Preorder and Flattening of Linked List
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List-Java version.xlsx
+++ b/Binary Search Tree/Java/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6839E896-880E-4CC7-BA2C-25F619151CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C723883-1637-4D8E-9D84-67B53D2CB32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="49">
   <si>
     <t>Question No</t>
   </si>
@@ -164,6 +164,38 @@
   </si>
   <si>
     <t>Construct Binary Tree from Preorder and Inorder Traversal</t>
+  </si>
+  <si>
+    <r>
+      <t>Binary Tree Inorder Traversal(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Morris Traversal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Binary Tree Preorder Traversal-(Morris Traversal)</t>
+  </si>
+  <si>
+    <t>Flatten Binary Tree to Linked List</t>
   </si>
 </sst>
 </file>
@@ -581,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:E29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,16 +1081,55 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="5"/>
+      <c r="A30" s="1">
+        <v>94</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="5"/>
+      <c r="A31" s="1">
+        <v>144</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="5"/>
+      <c r="A32" s="1">
+        <v>114</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>

</xml_diff>